<commit_message>
Added Bass diffusion structure
Added Bass diffusion model to represent implementation of CHL intervention
</commit_message>
<xml_diff>
--- a/Data/Combined activities and dose by month and community.xlsx
+++ b/Data/Combined activities and dose by month and community.xlsx
@@ -1,37 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psh2020/Documents/Models/CHL-Food-Systems/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psh2020/Documents/Models/CHLFS-intervention/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48FB43F-8AB5-9B4E-AE05-81739390B45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C8A820-02A5-0D40-80E2-69054E6C5354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="28780" windowHeight="14780" xr2:uid="{465B0F9F-F87E-4754-B96E-A920DA48AE03}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="28940" windowHeight="16900" activeTab="2" xr2:uid="{465B0F9F-F87E-4754-B96E-A920DA48AE03}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Implementation Curves" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$49</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$49:$AC$49</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$49</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$49:$AC$49</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$B$50</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$B$50:$AC$50</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$C$48:$AC$48</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$50</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$50:$AC$50</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$48:$AC$48</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$49</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$B$49:$AC$49</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$50</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$50:$AC$50</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$C$48:$AC$48</definedName>
     <definedName name="ExternalData_1" localSheetId="1">Sheet1!$A$1:$AD$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -67,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="18">
   <si>
     <t>Number of activities and dose by community by month</t>
   </si>
@@ -119,6 +105,9 @@
   <si>
     <t>Community 111</t>
   </si>
+  <si>
+    <t>variable</t>
+  </si>
 </sst>
 </file>
 
@@ -167,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -175,6 +164,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3071,7 +3063,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{92C27332-EC98-9A40-8F20-D95FA26076CF}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3082,7 +3074,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8682404" cy="6288942"/>
+    <xdr:ext cx="8662737" cy="6283158"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3116,9 +3108,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3156,7 +3148,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3262,7 +3254,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3404,7 +3396,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3414,8 +3406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B26D908-93C9-43B5-839A-2BCC95E4635B}">
   <dimension ref="A1:AD57"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:AD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3526,7 +3518,7 @@
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="5">
         <v>33</v>
       </c>
       <c r="B4" t="s">
@@ -3618,7 +3610,7 @@
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -3709,7 +3701,7 @@
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="5">
         <v>34</v>
       </c>
       <c r="B6" t="s">
@@ -3801,7 +3793,7 @@
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -3892,7 +3884,7 @@
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="5">
         <v>41</v>
       </c>
       <c r="B8" t="s">
@@ -3984,7 +3976,7 @@
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -4075,7 +4067,7 @@
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="5">
         <v>43</v>
       </c>
       <c r="B10" t="s">
@@ -4167,7 +4159,7 @@
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+      <c r="A11" s="5"/>
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -4258,7 +4250,7 @@
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="A12" s="5">
         <v>91</v>
       </c>
       <c r="B12" t="s">
@@ -4350,7 +4342,7 @@
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+      <c r="A13" s="5"/>
       <c r="B13" t="s">
         <v>5</v>
       </c>
@@ -4441,7 +4433,7 @@
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14" s="5">
         <v>92</v>
       </c>
       <c r="B14" t="s">
@@ -4533,7 +4525,7 @@
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
+      <c r="A15" s="5"/>
       <c r="B15" t="s">
         <v>5</v>
       </c>
@@ -4624,7 +4616,7 @@
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="A16" s="5">
         <v>101</v>
       </c>
       <c r="B16" t="s">
@@ -4716,7 +4708,7 @@
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
+      <c r="A17" s="5"/>
       <c r="B17" t="s">
         <v>5</v>
       </c>
@@ -4807,7 +4799,7 @@
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="A18" s="5">
         <v>103</v>
       </c>
       <c r="B18" t="s">
@@ -4899,7 +4891,7 @@
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
+      <c r="A19" s="5"/>
       <c r="B19" t="s">
         <v>5</v>
       </c>
@@ -4990,7 +4982,7 @@
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="A20" s="5">
         <v>111</v>
       </c>
       <c r="B20" t="s">
@@ -5082,7 +5074,7 @@
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
+      <c r="A21" s="5"/>
       <c r="B21" t="s">
         <v>5</v>
       </c>
@@ -5173,7 +5165,7 @@
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B22" t="s">
@@ -5265,7 +5257,7 @@
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
+      <c r="A23" s="5"/>
       <c r="B23" t="s">
         <v>5</v>
       </c>
@@ -7571,111 +7563,111 @@
         <v>8</v>
       </c>
       <c r="C49">
-        <f>C29</f>
+        <f t="shared" ref="C49:AC49" si="10">C29</f>
         <v>0</v>
       </c>
       <c r="D49">
-        <f>D29</f>
+        <f t="shared" si="10"/>
         <v>7.7519379844961239E-3</v>
       </c>
       <c r="E49">
-        <f>E29</f>
+        <f t="shared" si="10"/>
         <v>7.7519379844961239E-3</v>
       </c>
       <c r="F49">
-        <f>F29</f>
+        <f t="shared" si="10"/>
         <v>7.7519379844961239E-3</v>
       </c>
       <c r="G49">
-        <f>G29</f>
+        <f t="shared" si="10"/>
         <v>7.7519379844961239E-3</v>
       </c>
       <c r="H49">
-        <f>H29</f>
+        <f t="shared" si="10"/>
         <v>3.875968992248062E-2</v>
       </c>
       <c r="I49">
-        <f>I29</f>
+        <f t="shared" si="10"/>
         <v>6.9767441860465115E-2</v>
       </c>
       <c r="J49">
-        <f>J29</f>
+        <f t="shared" si="10"/>
         <v>9.3023255813953487E-2</v>
       </c>
       <c r="K49">
-        <f>K29</f>
+        <f t="shared" si="10"/>
         <v>0.10077519379844961</v>
       </c>
       <c r="L49">
-        <f>L29</f>
+        <f t="shared" si="10"/>
         <v>0.16279069767441862</v>
       </c>
       <c r="M49">
-        <f>M29</f>
+        <f t="shared" si="10"/>
         <v>0.20155038759689922</v>
       </c>
       <c r="N49">
-        <f>N29</f>
+        <f t="shared" si="10"/>
         <v>0.20155038759689922</v>
       </c>
       <c r="O49">
-        <f>O29</f>
+        <f t="shared" si="10"/>
         <v>0.23255813953488372</v>
       </c>
       <c r="P49">
-        <f>P29</f>
+        <f t="shared" si="10"/>
         <v>0.29457364341085274</v>
       </c>
       <c r="Q49">
-        <f>Q29</f>
+        <f t="shared" si="10"/>
         <v>0.35658914728682173</v>
       </c>
       <c r="R49">
-        <f>R29</f>
+        <f t="shared" si="10"/>
         <v>0.41860465116279072</v>
       </c>
       <c r="S49">
-        <f>S29</f>
+        <f t="shared" si="10"/>
         <v>0.48837209302325579</v>
       </c>
       <c r="T49">
-        <f>T29</f>
+        <f t="shared" si="10"/>
         <v>0.55038759689922478</v>
       </c>
       <c r="U49">
-        <f>U29</f>
+        <f t="shared" si="10"/>
         <v>0.61240310077519378</v>
       </c>
       <c r="V49">
-        <f>V29</f>
+        <f t="shared" si="10"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="W49">
-        <f>W29</f>
+        <f t="shared" si="10"/>
         <v>0.7441860465116279</v>
       </c>
       <c r="X49">
-        <f>X29</f>
+        <f t="shared" si="10"/>
         <v>0.80620155038759689</v>
       </c>
       <c r="Y49">
-        <f>Y29</f>
+        <f t="shared" si="10"/>
         <v>0.86821705426356588</v>
       </c>
       <c r="Z49">
-        <f>Z29</f>
+        <f t="shared" si="10"/>
         <v>0.90697674418604646</v>
       </c>
       <c r="AA49">
-        <f>AA29</f>
+        <f t="shared" si="10"/>
         <v>0.94573643410852715</v>
       </c>
       <c r="AB49">
-        <f>AB29</f>
+        <f t="shared" si="10"/>
         <v>0.98449612403100772</v>
       </c>
       <c r="AC49">
-        <f>AC29</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
@@ -7688,107 +7680,107 @@
         <v>0</v>
       </c>
       <c r="D50">
-        <f t="shared" ref="D50:AC50" si="10">D31</f>
+        <f t="shared" ref="D50:AC50" si="11">D31</f>
         <v>4.5977011494252873E-2</v>
       </c>
       <c r="E50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.5977011494252873E-2</v>
       </c>
       <c r="F50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.5977011494252873E-2</v>
       </c>
       <c r="G50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.5977011494252873E-2</v>
       </c>
       <c r="H50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.5977011494252873E-2</v>
       </c>
       <c r="I50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.5977011494252873E-2</v>
       </c>
       <c r="J50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.1954022988505746E-2</v>
       </c>
       <c r="K50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.11494252873563218</v>
       </c>
       <c r="L50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.16091954022988506</v>
       </c>
       <c r="M50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.19540229885057472</v>
       </c>
       <c r="N50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.19540229885057472</v>
       </c>
       <c r="O50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.19540229885057472</v>
       </c>
       <c r="P50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.28735632183908044</v>
       </c>
       <c r="Q50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.28735632183908044</v>
       </c>
       <c r="R50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.28735632183908044</v>
       </c>
       <c r="S50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.28735632183908044</v>
       </c>
       <c r="T50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.28735632183908044</v>
       </c>
       <c r="U50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.28735632183908044</v>
       </c>
       <c r="V50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.37931034482758619</v>
       </c>
       <c r="W50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.47126436781609193</v>
       </c>
       <c r="X50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.56321839080459768</v>
       </c>
       <c r="Y50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="Z50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.77011494252873558</v>
       </c>
       <c r="AA50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.87356321839080464</v>
       </c>
       <c r="AB50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.97701149425287359</v>
       </c>
       <c r="AC50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -7801,107 +7793,107 @@
         <v>1.8018018018018018E-2</v>
       </c>
       <c r="D51">
-        <f t="shared" ref="D51:AC51" si="11">D33</f>
+        <f t="shared" ref="D51:AC51" si="12">D33</f>
         <v>1.8018018018018018E-2</v>
       </c>
       <c r="E51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.7027027027027029E-2</v>
       </c>
       <c r="F51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4.5045045045045043E-2</v>
       </c>
       <c r="G51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.4054054054054057E-2</v>
       </c>
       <c r="H51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>8.1081081081081086E-2</v>
       </c>
       <c r="I51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9.0090090090090086E-2</v>
       </c>
       <c r="J51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.10810810810810811</v>
       </c>
       <c r="K51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.11711711711711711</v>
       </c>
       <c r="L51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.16216216216216217</v>
       </c>
       <c r="M51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.18018018018018017</v>
       </c>
       <c r="N51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.1891891891891892</v>
       </c>
       <c r="O51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.23423423423423423</v>
       </c>
       <c r="P51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.28828828828828829</v>
       </c>
       <c r="Q51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.36036036036036034</v>
       </c>
       <c r="R51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.42342342342342343</v>
       </c>
       <c r="S51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.49549549549549549</v>
       </c>
       <c r="T51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.55855855855855852</v>
       </c>
       <c r="U51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.63063063063063063</v>
       </c>
       <c r="V51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.70270270270270274</v>
       </c>
       <c r="W51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.7927927927927928</v>
       </c>
       <c r="X51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.83783783783783783</v>
       </c>
       <c r="Y51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.87387387387387383</v>
       </c>
       <c r="Z51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.91891891891891897</v>
       </c>
       <c r="AA51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.95495495495495497</v>
       </c>
       <c r="AB51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="AC51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -7914,107 +7906,107 @@
         <v>8.1967213114754103E-3</v>
       </c>
       <c r="D52">
-        <f t="shared" ref="D52:AC52" si="12">D35</f>
+        <f t="shared" ref="D52:AC52" si="13">D35</f>
         <v>8.1967213114754103E-3</v>
       </c>
       <c r="E52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.6393442622950821E-2</v>
       </c>
       <c r="F52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.4590163934426229E-2</v>
       </c>
       <c r="G52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.2786885245901641E-2</v>
       </c>
       <c r="H52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7.3770491803278687E-2</v>
       </c>
       <c r="I52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>8.1967213114754092E-2</v>
       </c>
       <c r="J52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.10655737704918032</v>
       </c>
       <c r="K52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.14754098360655737</v>
       </c>
       <c r="L52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.18852459016393441</v>
       </c>
       <c r="M52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.23770491803278687</v>
       </c>
       <c r="N52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.27868852459016391</v>
       </c>
       <c r="O52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.32786885245901637</v>
       </c>
       <c r="P52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.37704918032786883</v>
       </c>
       <c r="Q52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.4344262295081967</v>
       </c>
       <c r="R52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.49180327868852458</v>
       </c>
       <c r="S52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.59836065573770492</v>
       </c>
       <c r="T52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.67213114754098358</v>
       </c>
       <c r="U52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.74590163934426235</v>
       </c>
       <c r="V52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.81967213114754101</v>
       </c>
       <c r="W52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.86885245901639341</v>
       </c>
       <c r="X52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.89344262295081966</v>
       </c>
       <c r="Y52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.93442622950819676</v>
       </c>
       <c r="Z52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.97540983606557374</v>
       </c>
       <c r="AA52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.99180327868852458</v>
       </c>
       <c r="AB52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AC52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -8027,107 +8019,107 @@
         <v>5.434782608695652E-2</v>
       </c>
       <c r="D53">
-        <f t="shared" ref="D53:AC53" si="13">D37</f>
+        <f t="shared" ref="D53:AC53" si="14">D37</f>
         <v>6.5217391304347824E-2</v>
       </c>
       <c r="E53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.10869565217391304</v>
       </c>
       <c r="F53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="G53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="H53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="I53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="J53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="K53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.30434782608695654</v>
       </c>
       <c r="L53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.30434782608695654</v>
       </c>
       <c r="M53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.30434782608695654</v>
       </c>
       <c r="N53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.30434782608695654</v>
       </c>
       <c r="O53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.35869565217391303</v>
       </c>
       <c r="P53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.42391304347826086</v>
       </c>
       <c r="Q53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.51086956521739135</v>
       </c>
       <c r="R53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.57608695652173914</v>
       </c>
       <c r="S53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.65217391304347827</v>
       </c>
       <c r="T53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.65217391304347827</v>
       </c>
       <c r="U53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.70652173913043481</v>
       </c>
       <c r="V53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.73913043478260865</v>
       </c>
       <c r="W53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.78260869565217395</v>
       </c>
       <c r="X53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.81521739130434778</v>
       </c>
       <c r="Y53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.85869565217391308</v>
       </c>
       <c r="Z53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.93478260869565222</v>
       </c>
       <c r="AA53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.96739130434782605</v>
       </c>
       <c r="AB53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.98913043478260865</v>
       </c>
       <c r="AC53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
@@ -8140,107 +8132,107 @@
         <v>1.6129032258064516E-2</v>
       </c>
       <c r="D54">
-        <f t="shared" ref="D54:AC54" si="14">D39</f>
+        <f t="shared" ref="D54:AC54" si="15">D39</f>
         <v>1.6129032258064516E-2</v>
       </c>
       <c r="E54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3.2258064516129031E-2</v>
       </c>
       <c r="F54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9.6774193548387094E-2</v>
       </c>
       <c r="G54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9.6774193548387094E-2</v>
       </c>
       <c r="H54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9.6774193548387094E-2</v>
       </c>
       <c r="I54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9.6774193548387094E-2</v>
       </c>
       <c r="J54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9.6774193548387094E-2</v>
       </c>
       <c r="K54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.27419354838709675</v>
       </c>
       <c r="L54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.27419354838709675</v>
       </c>
       <c r="M54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.27419354838709675</v>
       </c>
       <c r="N54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.27419354838709675</v>
       </c>
       <c r="O54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.35483870967741937</v>
       </c>
       <c r="P54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.38709677419354838</v>
       </c>
       <c r="Q54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.43548387096774194</v>
       </c>
       <c r="R54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.5</v>
       </c>
       <c r="S54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.66129032258064513</v>
       </c>
       <c r="T54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.66129032258064513</v>
       </c>
       <c r="U54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.69354838709677424</v>
       </c>
       <c r="V54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.69354838709677424</v>
       </c>
       <c r="W54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.70967741935483875</v>
       </c>
       <c r="X54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.74193548387096775</v>
       </c>
       <c r="Y54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.80645161290322576</v>
       </c>
       <c r="Z54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.85483870967741937</v>
       </c>
       <c r="AA54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.95161290322580649</v>
       </c>
       <c r="AB54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="AC54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -8253,107 +8245,107 @@
         <v>1.3953488372093023E-2</v>
       </c>
       <c r="D55">
-        <f t="shared" ref="D55:AC55" si="15">D41</f>
+        <f t="shared" ref="D55:AC55" si="16">D41</f>
         <v>2.3255813953488372E-2</v>
       </c>
       <c r="E55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3.7209302325581395E-2</v>
       </c>
       <c r="F55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7.9069767441860464E-2</v>
       </c>
       <c r="G55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.11162790697674418</v>
       </c>
       <c r="H55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.13023255813953488</v>
       </c>
       <c r="I55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.15348837209302327</v>
       </c>
       <c r="J55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.17209302325581396</v>
       </c>
       <c r="K55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.18604651162790697</v>
       </c>
       <c r="L55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.26511627906976742</v>
       </c>
       <c r="M55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.32558139534883723</v>
       </c>
       <c r="N55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.39534883720930231</v>
       </c>
       <c r="O55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.46511627906976744</v>
       </c>
       <c r="P55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.52093023255813953</v>
       </c>
       <c r="Q55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.59069767441860466</v>
       </c>
       <c r="R55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.66976744186046511</v>
       </c>
       <c r="S55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.71627906976744182</v>
       </c>
       <c r="T55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.75813953488372088</v>
       </c>
       <c r="U55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.79069767441860461</v>
       </c>
       <c r="V55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.80930232558139537</v>
       </c>
       <c r="W55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.82325581395348835</v>
       </c>
       <c r="X55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.86046511627906974</v>
       </c>
       <c r="Y55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.90697674418604646</v>
       </c>
       <c r="Z55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.93488372093023253</v>
       </c>
       <c r="AA55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.94883720930232562</v>
       </c>
       <c r="AB55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.98604651162790702</v>
       </c>
       <c r="AC55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
     </row>
@@ -8366,107 +8358,107 @@
         <v>2.5974025974025976E-2</v>
       </c>
       <c r="D56">
-        <f t="shared" ref="D56:AC56" si="16">D43</f>
+        <f t="shared" ref="D56:AC56" si="17">D43</f>
         <v>3.896103896103896E-2</v>
       </c>
       <c r="E56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5.1948051948051951E-2</v>
       </c>
       <c r="F56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>6.4935064935064929E-2</v>
       </c>
       <c r="G56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7.792207792207792E-2</v>
       </c>
       <c r="H56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="I56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.1038961038961039</v>
       </c>
       <c r="J56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.1038961038961039</v>
       </c>
       <c r="K56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.12987012987012986</v>
       </c>
       <c r="L56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="M56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.25974025974025972</v>
       </c>
       <c r="N56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.31168831168831168</v>
       </c>
       <c r="O56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.37662337662337664</v>
       </c>
       <c r="P56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.46753246753246752</v>
       </c>
       <c r="Q56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.53246753246753242</v>
       </c>
       <c r="R56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.5714285714285714</v>
       </c>
       <c r="S56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.62337662337662336</v>
       </c>
       <c r="T56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.64935064935064934</v>
       </c>
       <c r="U56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.68831168831168832</v>
       </c>
       <c r="V56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="W56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.81818181818181823</v>
       </c>
       <c r="X56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.87012987012987009</v>
       </c>
       <c r="Y56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.93506493506493504</v>
       </c>
       <c r="Z56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.94805194805194803</v>
       </c>
       <c r="AA56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.94805194805194803</v>
       </c>
       <c r="AB56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="AC56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
@@ -8479,107 +8471,107 @@
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" ref="D57:AC57" si="17">D45</f>
+        <f t="shared" ref="D57:AC57" si="18">D45</f>
         <v>2.0618556701030927E-2</v>
       </c>
       <c r="E57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.0618556701030927E-2</v>
       </c>
       <c r="F57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.0618556701030927E-2</v>
       </c>
       <c r="G57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.0618556701030927E-2</v>
       </c>
       <c r="H57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.0618556701030927E-2</v>
       </c>
       <c r="I57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>4.1237113402061855E-2</v>
       </c>
       <c r="J57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>4.1237113402061855E-2</v>
       </c>
       <c r="K57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>7.2164948453608241E-2</v>
       </c>
       <c r="L57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9.2783505154639179E-2</v>
       </c>
       <c r="M57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9.2783505154639179E-2</v>
       </c>
       <c r="N57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.10309278350515463</v>
       </c>
       <c r="O57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.17525773195876287</v>
       </c>
       <c r="P57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.21649484536082475</v>
       </c>
       <c r="Q57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.25773195876288657</v>
       </c>
       <c r="R57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.34020618556701032</v>
       </c>
       <c r="S57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.41237113402061853</v>
       </c>
       <c r="T57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.44329896907216493</v>
       </c>
       <c r="U57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.47422680412371132</v>
       </c>
       <c r="V57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.55670103092783507</v>
       </c>
       <c r="W57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.65979381443298968</v>
       </c>
       <c r="X57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.73195876288659789</v>
       </c>
       <c r="Y57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.79381443298969068</v>
       </c>
       <c r="Z57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.85567010309278346</v>
       </c>
       <c r="AA57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.91752577319587625</v>
       </c>
       <c r="AB57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.95876288659793818</v>
       </c>
       <c r="AC57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
     </row>
@@ -8599,4 +8591,1713 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61596CDF-6616-8A40-83AA-ADD3011288D5}">
+  <dimension ref="A1:AC19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+      <c r="Z1">
+        <v>24</v>
+      </c>
+      <c r="AA1">
+        <v>25</v>
+      </c>
+      <c r="AB1">
+        <v>26</v>
+      </c>
+      <c r="AC1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>8</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>4</v>
+      </c>
+      <c r="P2">
+        <v>8</v>
+      </c>
+      <c r="Q2">
+        <v>8</v>
+      </c>
+      <c r="R2">
+        <v>8</v>
+      </c>
+      <c r="S2">
+        <v>9</v>
+      </c>
+      <c r="T2">
+        <v>8</v>
+      </c>
+      <c r="U2">
+        <v>8</v>
+      </c>
+      <c r="V2">
+        <v>7</v>
+      </c>
+      <c r="W2">
+        <v>10</v>
+      </c>
+      <c r="X2">
+        <v>8</v>
+      </c>
+      <c r="Y2">
+        <v>8</v>
+      </c>
+      <c r="Z2">
+        <v>5</v>
+      </c>
+      <c r="AA2">
+        <v>5</v>
+      </c>
+      <c r="AB2">
+        <v>5</v>
+      </c>
+      <c r="AC2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.33</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1.6825000000000001</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>1.25</v>
+      </c>
+      <c r="K3">
+        <v>0.33</v>
+      </c>
+      <c r="L3">
+        <v>8.9280000000000008</v>
+      </c>
+      <c r="M3">
+        <v>8.2263999999999999</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>2.67</v>
+      </c>
+      <c r="P3">
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <v>4.33</v>
+      </c>
+      <c r="R3">
+        <v>4.33</v>
+      </c>
+      <c r="S3">
+        <v>6.64</v>
+      </c>
+      <c r="T3">
+        <v>3.99</v>
+      </c>
+      <c r="U3">
+        <v>3.99</v>
+      </c>
+      <c r="V3">
+        <v>3.66</v>
+      </c>
+      <c r="W3">
+        <v>7.75</v>
+      </c>
+      <c r="X3">
+        <v>4.74</v>
+      </c>
+      <c r="Y3">
+        <v>4.74</v>
+      </c>
+      <c r="Z3">
+        <v>2.4</v>
+      </c>
+      <c r="AA3">
+        <v>3.08</v>
+      </c>
+      <c r="AB3">
+        <v>2.74</v>
+      </c>
+      <c r="AC3">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>8</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>8</v>
+      </c>
+      <c r="W4">
+        <v>8</v>
+      </c>
+      <c r="X4">
+        <v>8</v>
+      </c>
+      <c r="Y4">
+        <v>9</v>
+      </c>
+      <c r="Z4">
+        <v>9</v>
+      </c>
+      <c r="AA4">
+        <v>9</v>
+      </c>
+      <c r="AB4">
+        <v>9</v>
+      </c>
+      <c r="AC4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>3.7109999999999999</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>3.32</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1.66</v>
+      </c>
+      <c r="M5">
+        <v>1.33</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>4.2312000000000003</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>4.4640000000000004</v>
+      </c>
+      <c r="W5">
+        <v>3.99</v>
+      </c>
+      <c r="X5">
+        <v>4.33</v>
+      </c>
+      <c r="Y5">
+        <v>5.33</v>
+      </c>
+      <c r="Z5">
+        <v>5.33</v>
+      </c>
+      <c r="AA5">
+        <v>5.33</v>
+      </c>
+      <c r="AB5">
+        <v>5.67</v>
+      </c>
+      <c r="AC5">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <v>6</v>
+      </c>
+      <c r="Q6">
+        <v>8</v>
+      </c>
+      <c r="R6">
+        <v>7</v>
+      </c>
+      <c r="S6">
+        <v>8</v>
+      </c>
+      <c r="T6">
+        <v>7</v>
+      </c>
+      <c r="U6">
+        <v>8</v>
+      </c>
+      <c r="V6">
+        <v>8</v>
+      </c>
+      <c r="W6">
+        <v>10</v>
+      </c>
+      <c r="X6">
+        <v>5</v>
+      </c>
+      <c r="Y6">
+        <v>4</v>
+      </c>
+      <c r="Z6">
+        <v>5</v>
+      </c>
+      <c r="AA6">
+        <v>4</v>
+      </c>
+      <c r="AB6">
+        <v>5</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>1.2857000000000001</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0.4</v>
+      </c>
+      <c r="F7">
+        <v>1.67</v>
+      </c>
+      <c r="G7">
+        <v>0.7</v>
+      </c>
+      <c r="H7">
+        <v>1.53</v>
+      </c>
+      <c r="I7">
+        <v>0.33</v>
+      </c>
+      <c r="J7">
+        <v>0.66</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>3.3172000000000001</v>
+      </c>
+      <c r="M7">
+        <v>1.47</v>
+      </c>
+      <c r="N7">
+        <v>1.34</v>
+      </c>
+      <c r="O7">
+        <v>4.68</v>
+      </c>
+      <c r="P7">
+        <v>4.34</v>
+      </c>
+      <c r="Q7">
+        <v>5.01</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7">
+        <v>6.8651999999999997</v>
+      </c>
+      <c r="T7">
+        <v>7.09</v>
+      </c>
+      <c r="U7">
+        <v>4.59</v>
+      </c>
+      <c r="V7">
+        <v>5.34</v>
+      </c>
+      <c r="W7">
+        <v>6.1449999999999996</v>
+      </c>
+      <c r="X7">
+        <v>3.32</v>
+      </c>
+      <c r="Y7">
+        <v>4.01</v>
+      </c>
+      <c r="Z7">
+        <v>6.02</v>
+      </c>
+      <c r="AA7">
+        <v>5.33</v>
+      </c>
+      <c r="AB7">
+        <v>4.67</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <v>6</v>
+      </c>
+      <c r="P8">
+        <v>6</v>
+      </c>
+      <c r="Q8">
+        <v>7</v>
+      </c>
+      <c r="R8">
+        <v>7</v>
+      </c>
+      <c r="S8">
+        <v>13</v>
+      </c>
+      <c r="T8">
+        <v>9</v>
+      </c>
+      <c r="U8">
+        <v>9</v>
+      </c>
+      <c r="V8">
+        <v>9</v>
+      </c>
+      <c r="W8">
+        <v>6</v>
+      </c>
+      <c r="X8">
+        <v>3</v>
+      </c>
+      <c r="Y8">
+        <v>5</v>
+      </c>
+      <c r="Z8">
+        <v>5</v>
+      </c>
+      <c r="AA8">
+        <v>2</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.48</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0.2475</v>
+      </c>
+      <c r="H9">
+        <v>3.2475000000000001</v>
+      </c>
+      <c r="I9">
+        <v>0.2475</v>
+      </c>
+      <c r="J9">
+        <v>1.66</v>
+      </c>
+      <c r="K9">
+        <v>5.67</v>
+      </c>
+      <c r="L9">
+        <v>4.5632999999999999</v>
+      </c>
+      <c r="M9">
+        <v>4.84</v>
+      </c>
+      <c r="N9">
+        <v>5.01</v>
+      </c>
+      <c r="O9">
+        <v>6.36</v>
+      </c>
+      <c r="P9">
+        <v>4.68</v>
+      </c>
+      <c r="Q9">
+        <v>4.68</v>
+      </c>
+      <c r="R9">
+        <v>4.1675000000000004</v>
+      </c>
+      <c r="S9">
+        <v>8.9412000000000003</v>
+      </c>
+      <c r="T9">
+        <v>5.4550000000000001</v>
+      </c>
+      <c r="U9">
+        <v>5.6448</v>
+      </c>
+      <c r="V9">
+        <v>6.1406999999999998</v>
+      </c>
+      <c r="W9">
+        <v>2.5270999999999999</v>
+      </c>
+      <c r="X9">
+        <v>1.65</v>
+      </c>
+      <c r="Y9">
+        <v>2.3605</v>
+      </c>
+      <c r="Z9">
+        <v>2.5024999999999999</v>
+      </c>
+      <c r="AA9">
+        <v>1.33</v>
+      </c>
+      <c r="AB9">
+        <v>0.33</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>12</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>5</v>
+      </c>
+      <c r="P10">
+        <v>6</v>
+      </c>
+      <c r="Q10">
+        <v>8</v>
+      </c>
+      <c r="R10">
+        <v>6</v>
+      </c>
+      <c r="S10">
+        <v>7</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>5</v>
+      </c>
+      <c r="V10">
+        <v>3</v>
+      </c>
+      <c r="W10">
+        <v>4</v>
+      </c>
+      <c r="X10">
+        <v>3</v>
+      </c>
+      <c r="Y10">
+        <v>4</v>
+      </c>
+      <c r="Z10">
+        <v>7</v>
+      </c>
+      <c r="AA10">
+        <v>3</v>
+      </c>
+      <c r="AB10">
+        <v>2</v>
+      </c>
+      <c r="AC10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>91</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>3.97</v>
+      </c>
+      <c r="D11">
+        <v>0.67</v>
+      </c>
+      <c r="E11">
+        <v>2.1648999999999998</v>
+      </c>
+      <c r="F11">
+        <v>3.1709000000000001</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>7.7210000000000001</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>4.1547999999999998</v>
+      </c>
+      <c r="P11">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="Q11">
+        <v>6.3627000000000002</v>
+      </c>
+      <c r="R11">
+        <v>6.9660000000000002</v>
+      </c>
+      <c r="S11">
+        <v>7.1710000000000003</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>3.57</v>
+      </c>
+      <c r="V11">
+        <v>1.33</v>
+      </c>
+      <c r="W11">
+        <v>1.3591</v>
+      </c>
+      <c r="X11">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="Y11">
+        <v>1.4783999999999999</v>
+      </c>
+      <c r="Z11">
+        <v>3.3119999999999998</v>
+      </c>
+      <c r="AA11">
+        <v>3.8740000000000001</v>
+      </c>
+      <c r="AB11">
+        <v>1.33</v>
+      </c>
+      <c r="AC11">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>92</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>11</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>5</v>
+      </c>
+      <c r="P12">
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <v>3</v>
+      </c>
+      <c r="R12">
+        <v>4</v>
+      </c>
+      <c r="S12">
+        <v>10</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>2</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12">
+        <v>2</v>
+      </c>
+      <c r="Y12">
+        <v>4</v>
+      </c>
+      <c r="Z12">
+        <v>3</v>
+      </c>
+      <c r="AA12">
+        <v>6</v>
+      </c>
+      <c r="AB12">
+        <v>3</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>92</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>0.67</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0.67</v>
+      </c>
+      <c r="F13">
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>8.5869999999999997</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>3.5828000000000002</v>
+      </c>
+      <c r="P13">
+        <v>5</v>
+      </c>
+      <c r="Q13">
+        <v>1.2988999999999999</v>
+      </c>
+      <c r="R13">
+        <v>3.34</v>
+      </c>
+      <c r="S13">
+        <v>6.03</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="X13">
+        <v>1.84</v>
+      </c>
+      <c r="Y13">
+        <v>4.6355000000000004</v>
+      </c>
+      <c r="Z13">
+        <v>0.8427</v>
+      </c>
+      <c r="AA13">
+        <v>6.0227000000000004</v>
+      </c>
+      <c r="AB13">
+        <v>2.4420000000000002</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>101</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>3</v>
+      </c>
+      <c r="L14">
+        <v>17</v>
+      </c>
+      <c r="M14">
+        <v>13</v>
+      </c>
+      <c r="N14">
+        <v>15</v>
+      </c>
+      <c r="O14">
+        <v>15</v>
+      </c>
+      <c r="P14">
+        <v>12</v>
+      </c>
+      <c r="Q14">
+        <v>15</v>
+      </c>
+      <c r="R14">
+        <v>17</v>
+      </c>
+      <c r="S14">
+        <v>10</v>
+      </c>
+      <c r="T14">
+        <v>9</v>
+      </c>
+      <c r="U14">
+        <v>7</v>
+      </c>
+      <c r="V14">
+        <v>4</v>
+      </c>
+      <c r="W14">
+        <v>3</v>
+      </c>
+      <c r="X14">
+        <v>8</v>
+      </c>
+      <c r="Y14">
+        <v>10</v>
+      </c>
+      <c r="Z14">
+        <v>6</v>
+      </c>
+      <c r="AA14">
+        <v>3</v>
+      </c>
+      <c r="AB14">
+        <v>8</v>
+      </c>
+      <c r="AC14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>101</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>1.66</v>
+      </c>
+      <c r="D15">
+        <v>3.33</v>
+      </c>
+      <c r="E15">
+        <v>3.835</v>
+      </c>
+      <c r="F15">
+        <v>6.7525000000000004</v>
+      </c>
+      <c r="G15">
+        <v>5.99</v>
+      </c>
+      <c r="H15">
+        <v>4.165</v>
+      </c>
+      <c r="I15">
+        <v>3.3650000000000002</v>
+      </c>
+      <c r="J15">
+        <v>1.665</v>
+      </c>
+      <c r="K15">
+        <v>1.2524999999999999</v>
+      </c>
+      <c r="L15">
+        <v>14.986499999999999</v>
+      </c>
+      <c r="M15">
+        <v>10.88</v>
+      </c>
+      <c r="N15">
+        <v>6.9348000000000001</v>
+      </c>
+      <c r="O15">
+        <v>9.6395</v>
+      </c>
+      <c r="P15">
+        <v>10.956</v>
+      </c>
+      <c r="Q15">
+        <v>12.3185</v>
+      </c>
+      <c r="R15">
+        <v>17.310700000000001</v>
+      </c>
+      <c r="S15">
+        <v>6.6755000000000004</v>
+      </c>
+      <c r="T15">
+        <v>7.8419999999999996</v>
+      </c>
+      <c r="U15">
+        <v>4.9180000000000001</v>
+      </c>
+      <c r="V15">
+        <v>3.6017999999999999</v>
+      </c>
+      <c r="W15">
+        <v>1.3959999999999999</v>
+      </c>
+      <c r="X15">
+        <v>3.7723</v>
+      </c>
+      <c r="Y15">
+        <v>8.2215000000000007</v>
+      </c>
+      <c r="Z15">
+        <v>4.2530000000000001</v>
+      </c>
+      <c r="AA15">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="AB15">
+        <v>5.2853000000000003</v>
+      </c>
+      <c r="AC15">
+        <v>2.8424999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>103</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>4</v>
+      </c>
+      <c r="M16">
+        <v>6</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+      <c r="O16">
+        <v>5</v>
+      </c>
+      <c r="P16">
+        <v>7</v>
+      </c>
+      <c r="Q16">
+        <v>5</v>
+      </c>
+      <c r="R16">
+        <v>3</v>
+      </c>
+      <c r="S16">
+        <v>4</v>
+      </c>
+      <c r="T16">
+        <v>2</v>
+      </c>
+      <c r="U16">
+        <v>3</v>
+      </c>
+      <c r="V16">
+        <v>2</v>
+      </c>
+      <c r="W16">
+        <v>8</v>
+      </c>
+      <c r="X16">
+        <v>4</v>
+      </c>
+      <c r="Y16">
+        <v>5</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>4</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>103</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>1.33</v>
+      </c>
+      <c r="D17">
+        <v>0.33</v>
+      </c>
+      <c r="E17">
+        <v>0.33</v>
+      </c>
+      <c r="F17">
+        <v>0.33</v>
+      </c>
+      <c r="G17">
+        <v>0.33</v>
+      </c>
+      <c r="H17">
+        <v>0.33</v>
+      </c>
+      <c r="I17">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>1.165</v>
+      </c>
+      <c r="L17">
+        <v>3.01</v>
+      </c>
+      <c r="M17">
+        <v>5.923</v>
+      </c>
+      <c r="N17">
+        <v>2.056</v>
+      </c>
+      <c r="O17">
+        <v>3.1339999999999999</v>
+      </c>
+      <c r="P17">
+        <v>4.4188000000000001</v>
+      </c>
+      <c r="Q17">
+        <v>8.0820000000000007</v>
+      </c>
+      <c r="R17">
+        <v>3</v>
+      </c>
+      <c r="S17">
+        <v>2.6432000000000002</v>
+      </c>
+      <c r="T17">
+        <v>1.2</v>
+      </c>
+      <c r="U17">
+        <v>1.464</v>
+      </c>
+      <c r="V17">
+        <v>4</v>
+      </c>
+      <c r="W17">
+        <v>5.99</v>
+      </c>
+      <c r="X17">
+        <v>2.871</v>
+      </c>
+      <c r="Y17">
+        <v>3.33</v>
+      </c>
+      <c r="Z17">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>2.2040000000000002</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>111</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>7</v>
+      </c>
+      <c r="P18">
+        <v>4</v>
+      </c>
+      <c r="Q18">
+        <v>4</v>
+      </c>
+      <c r="R18">
+        <v>8</v>
+      </c>
+      <c r="S18">
+        <v>7</v>
+      </c>
+      <c r="T18">
+        <v>3</v>
+      </c>
+      <c r="U18">
+        <v>3</v>
+      </c>
+      <c r="V18">
+        <v>8</v>
+      </c>
+      <c r="W18">
+        <v>10</v>
+      </c>
+      <c r="X18">
+        <v>7</v>
+      </c>
+      <c r="Y18">
+        <v>6</v>
+      </c>
+      <c r="Z18">
+        <v>6</v>
+      </c>
+      <c r="AA18">
+        <v>6</v>
+      </c>
+      <c r="AB18">
+        <v>4</v>
+      </c>
+      <c r="AC18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>111</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0.66</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0.66</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>2.8475000000000001</v>
+      </c>
+      <c r="L19">
+        <v>2.68</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0.67</v>
+      </c>
+      <c r="O19">
+        <v>9.33</v>
+      </c>
+      <c r="P19">
+        <v>2.67</v>
+      </c>
+      <c r="Q19">
+        <v>2.67</v>
+      </c>
+      <c r="R19">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="S19">
+        <v>6.1875</v>
+      </c>
+      <c r="T19">
+        <v>1.66</v>
+      </c>
+      <c r="U19">
+        <v>0.99</v>
+      </c>
+      <c r="V19">
+        <v>3.31</v>
+      </c>
+      <c r="W19">
+        <v>4.5688000000000004</v>
+      </c>
+      <c r="X19">
+        <v>2.4828000000000001</v>
+      </c>
+      <c r="Y19">
+        <v>1.7426999999999999</v>
+      </c>
+      <c r="Z19">
+        <v>1.7031000000000001</v>
+      </c>
+      <c r="AA19">
+        <v>2.02</v>
+      </c>
+      <c r="AB19">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="AC19">
+        <v>1.66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>